<commit_message>
Make sheet writer only work to single sheet, not to all.
</commit_message>
<xml_diff>
--- a/excel/test/user.xlsx
+++ b/excel/test/user.xlsx
@@ -37,7 +37,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -48,19 +48,11 @@
     <font>
       <name val="Arial"/>
       <sz val="12.0"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Arial"/>
       <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="4">
@@ -95,26 +87,29 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -134,35 +129,35 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" t="s" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="5">
+      <c r="A2" t="n" s="1">
         <v>18.0</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="5">
+      <c r="A3" t="n" s="1">
         <v>18.0</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" t="s" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>